<commit_message>
Updated the Misclassification file.
</commit_message>
<xml_diff>
--- a/Misclassifications.xlsx
+++ b/Misclassifications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\meng-ucalgary\ensf-612-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayod\OneDrive\Desktop\master\Uoc\612_BigData\PROJECT STUFF\ensf-612-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E695D0F-DDA2-49CE-B0C8-58147CAE31FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F899B18-A622-4E6B-A27C-5AC83683E033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2985" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="423">
   <si>
     <t>file_id</t>
   </si>
@@ -1089,16 +1089,226 @@
     <t>Layout could have caused it as Background and hence What</t>
   </si>
   <si>
-    <t>Some background about working of the slack commands is given</t>
-  </si>
-  <si>
-    <t>Edition, the might have caused it to get labelled as introduction</t>
-  </si>
-  <si>
-    <t>Introduction, getting started, and some background on first chapter</t>
-  </si>
-  <si>
-    <t>to be merged</t>
+    <t>Because the word "how" in the first sentence.</t>
+  </si>
+  <si>
+    <t>The model assumes instructions were being given</t>
+  </si>
+  <si>
+    <t>The model assumes "how"  because of the active word "forked".</t>
+  </si>
+  <si>
+    <t>Might be due to some words appearing to suggest instructions</t>
+  </si>
+  <si>
+    <t>The model intepretes some words to be instruction</t>
+  </si>
+  <si>
+    <t>The model probably missed the  "what" part of the section</t>
+  </si>
+  <si>
+    <t>Probably focused on the word "tested"</t>
+  </si>
+  <si>
+    <t>Intepreted the active words as instructions</t>
+  </si>
+  <si>
+    <t>A short reference was made to a folder during the instruction process</t>
+  </si>
+  <si>
+    <t>A few line intepreted as introduction</t>
+  </si>
+  <si>
+    <t>The model return none of te category. No words after the section heading.</t>
+  </si>
+  <si>
+    <t>Because of the presence of " src/folder"</t>
+  </si>
+  <si>
+    <t>Asumes instruction were also being given</t>
+  </si>
+  <si>
+    <t>Asumed some words relating to reference</t>
+  </si>
+  <si>
+    <t>The first sentence contains discriptive word.</t>
+  </si>
+  <si>
+    <t>Intepreted as a refrence by the model</t>
+  </si>
+  <si>
+    <t>The model sees the command line instructions and classified as "how"</t>
+  </si>
+  <si>
+    <t>Assumed the instruction to be an introduction</t>
+  </si>
+  <si>
+    <t>Did not classify. Might be due to short phrase</t>
+  </si>
+  <si>
+    <t>Classified based name and twiiter account appearing</t>
+  </si>
+  <si>
+    <t>Model did not classify</t>
+  </si>
+  <si>
+    <t>Probably because of short phrase</t>
+  </si>
+  <si>
+    <t>Model only focused on words indicating instructions</t>
+  </si>
+  <si>
+    <t>The model missed the explanation part of the section</t>
+  </si>
+  <si>
+    <t>The model probably spotted the date and intepreted it as "version"</t>
+  </si>
+  <si>
+    <t>Probably spotted "Amazon" as name thereby classifying as "who".</t>
+  </si>
+  <si>
+    <t>Assumed some of active words to be giving instructions</t>
+  </si>
+  <si>
+    <t>Providing explanation of integrating with IDEs was taken as "reference"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The model assumes the section is giving instructions </t>
+  </si>
+  <si>
+    <t>Got most classification right but couldn't understand some commad line argument</t>
+  </si>
+  <si>
+    <t>The model assumes the section is giving background information for the project.</t>
+  </si>
+  <si>
+    <t>The model assumes the section is giving more information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The model assumes the section is </t>
+  </si>
+  <si>
+    <t>Model couldn't classify as "others"</t>
+  </si>
+  <si>
+    <t>The model assumes the section is giving more infromation and related projects.</t>
+  </si>
+  <si>
+    <t>The model assumes section is giving installation instructions and is giving more information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The model assumes the section is giving instructions on how to use GitBook. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The model assumes the section is talking about the people behind the project. </t>
+  </si>
+  <si>
+    <t>This model assumes the section is giving more information.</t>
+  </si>
+  <si>
+    <t>The model ignored the section title</t>
+  </si>
+  <si>
+    <t>Models assumes some active words as passing instructions.</t>
+  </si>
+  <si>
+    <t>Spoted the name "Gabriel Falcao" and classified as "who"</t>
+  </si>
+  <si>
+    <t>Classified based on "we" and the url.</t>
+  </si>
+  <si>
+    <t>Might have classified based on the word "apply".</t>
+  </si>
+  <si>
+    <t>The model assumes the section is giving more information</t>
+  </si>
+  <si>
+    <t>The model assumes the section is providing multiple links that give more information.</t>
+  </si>
+  <si>
+    <t>The model assumes the section is providing more information. -  "…information on how to do so is here…"</t>
+  </si>
+  <si>
+    <t>Classified the instruction correctly</t>
+  </si>
+  <si>
+    <t>Asuumed the path to folder is "reference"</t>
+  </si>
+  <si>
+    <t>Classified correctly, returned blank because of the command line instruction</t>
+  </si>
+  <si>
+    <t>The model picked  6 after reading the "For more info…" sentence.</t>
+  </si>
+  <si>
+    <t>Classified wrongly probably because of "coming" word</t>
+  </si>
+  <si>
+    <t>Could not classify the title.</t>
+  </si>
+  <si>
+    <t>Assumed active words to be giving instructions</t>
+  </si>
+  <si>
+    <t>Excluded the "what" part of the section. Therby clasified as "what".</t>
+  </si>
+  <si>
+    <t>Asummed "example.com" as a reference.</t>
+  </si>
+  <si>
+    <t>Misclassified wrongly.</t>
+  </si>
+  <si>
+    <t>Asumedthe title to be giving instructions.</t>
+  </si>
+  <si>
+    <t>Omiited the "why" part of the section</t>
+  </si>
+  <si>
+    <t>Classified based on some explanatory words e.g "provides"</t>
+  </si>
+  <si>
+    <t>Some of the instructions were taken as "references"</t>
+  </si>
+  <si>
+    <t>The section mentioned the book name and the model classified it as refrence.</t>
+  </si>
+  <si>
+    <t>Got "what" right</t>
+  </si>
+  <si>
+    <t>Did not classify the section based on a very shor phrase.</t>
+  </si>
+  <si>
+    <t>Asuumed the url to be a "refrence"</t>
+  </si>
+  <si>
+    <t>Missed the "what" paer of the explanation</t>
+  </si>
+  <si>
+    <t>Intepreted tge reference to the link as part of the instructions</t>
+  </si>
+  <si>
+    <t>Classified the the url as "reference".</t>
+  </si>
+  <si>
+    <t>Missed the section probably because the title was not seperated</t>
+  </si>
+  <si>
+    <t>Missed the "why" part probably because alll the categories were emebedded in the whole section.</t>
+  </si>
+  <si>
+    <t>Might have read some version number as dates</t>
+  </si>
+  <si>
+    <t>Read the title as "references"</t>
+  </si>
+  <si>
+    <t>Read  some of the words e.g "slack.slash" as "references"</t>
+  </si>
+  <si>
+    <t>Assumed the first sentence to be an instruction.</t>
   </si>
 </sst>
 </file>
@@ -12633,24 +12843,24 @@
   <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D215" sqref="D215"/>
+      <selection activeCell="B204" sqref="B204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="40.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="40.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" hidden="1"/>
+    <col min="11" max="16384" width="8.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12679,7 +12889,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12706,10 +12916,10 @@
         <v>259</v>
       </c>
       <c r="I2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -12736,10 +12946,10 @@
         <v>259</v>
       </c>
       <c r="I3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -12766,10 +12976,10 @@
         <v>259</v>
       </c>
       <c r="I4" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -12799,7 +13009,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -12826,10 +13036,10 @@
         <v>259</v>
       </c>
       <c r="I6" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -12856,10 +13066,10 @@
         <v>259</v>
       </c>
       <c r="I7" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -12886,10 +13096,10 @@
         <v>259</v>
       </c>
       <c r="I8" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -12916,10 +13126,10 @@
         <v>259</v>
       </c>
       <c r="I9" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -12946,10 +13156,10 @@
         <v>259</v>
       </c>
       <c r="I10" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -12976,10 +13186,10 @@
         <v>259</v>
       </c>
       <c r="I11" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -13006,10 +13216,10 @@
         <v>259</v>
       </c>
       <c r="I12" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -13036,10 +13246,10 @@
         <v>259</v>
       </c>
       <c r="I13" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -13066,10 +13276,10 @@
         <v>259</v>
       </c>
       <c r="I14" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -13096,10 +13306,10 @@
         <v>259</v>
       </c>
       <c r="I15" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -13126,10 +13336,10 @@
         <v>259</v>
       </c>
       <c r="I16" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -13156,10 +13366,10 @@
         <v>259</v>
       </c>
       <c r="I17" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -13186,10 +13396,10 @@
         <v>259</v>
       </c>
       <c r="I18" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -13216,10 +13426,10 @@
         <v>259</v>
       </c>
       <c r="I19" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -13246,10 +13456,10 @@
         <v>259</v>
       </c>
       <c r="I20" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -13276,10 +13486,10 @@
         <v>259</v>
       </c>
       <c r="I21" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -13306,10 +13516,10 @@
         <v>259</v>
       </c>
       <c r="I22" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -13336,10 +13546,10 @@
         <v>259</v>
       </c>
       <c r="I23" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -13366,10 +13576,10 @@
         <v>259</v>
       </c>
       <c r="I24" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -13396,10 +13606,10 @@
         <v>259</v>
       </c>
       <c r="I25" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -13426,10 +13636,10 @@
         <v>259</v>
       </c>
       <c r="I26" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -13456,10 +13666,10 @@
         <v>259</v>
       </c>
       <c r="I27" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -13486,10 +13696,10 @@
         <v>259</v>
       </c>
       <c r="I28" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -13516,10 +13726,10 @@
         <v>259</v>
       </c>
       <c r="I29" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -13546,10 +13756,10 @@
         <v>259</v>
       </c>
       <c r="I30" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -13576,10 +13786,10 @@
         <v>259</v>
       </c>
       <c r="I31" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -13606,10 +13816,10 @@
         <v>259</v>
       </c>
       <c r="I32" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -13636,10 +13846,10 @@
         <v>259</v>
       </c>
       <c r="I33" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -13666,10 +13876,10 @@
         <v>259</v>
       </c>
       <c r="I34" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11</v>
       </c>
@@ -13696,10 +13906,10 @@
         <v>259</v>
       </c>
       <c r="I35" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -13726,10 +13936,10 @@
         <v>259</v>
       </c>
       <c r="I36" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>11</v>
       </c>
@@ -13756,10 +13966,10 @@
         <v>259</v>
       </c>
       <c r="I37" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>11</v>
       </c>
@@ -13786,10 +13996,10 @@
         <v>259</v>
       </c>
       <c r="I38" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
@@ -13816,10 +14026,10 @@
         <v>259</v>
       </c>
       <c r="I39" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11</v>
       </c>
@@ -13846,10 +14056,10 @@
         <v>259</v>
       </c>
       <c r="I40" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>11</v>
       </c>
@@ -13876,10 +14086,10 @@
         <v>259</v>
       </c>
       <c r="I41" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>11</v>
       </c>
@@ -13906,10 +14116,10 @@
         <v>259</v>
       </c>
       <c r="I42" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>11</v>
       </c>
@@ -13936,10 +14146,10 @@
         <v>259</v>
       </c>
       <c r="I43" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>11</v>
       </c>
@@ -13966,10 +14176,10 @@
         <v>259</v>
       </c>
       <c r="I44" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>11</v>
       </c>
@@ -13996,10 +14206,10 @@
         <v>259</v>
       </c>
       <c r="I45" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>11</v>
       </c>
@@ -14026,10 +14236,10 @@
         <v>259</v>
       </c>
       <c r="I46" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>11</v>
       </c>
@@ -14056,10 +14266,10 @@
         <v>259</v>
       </c>
       <c r="I47" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>11</v>
       </c>
@@ -14086,10 +14296,10 @@
         <v>259</v>
       </c>
       <c r="I48" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>11</v>
       </c>
@@ -14116,10 +14326,10 @@
         <v>259</v>
       </c>
       <c r="I49" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>11</v>
       </c>
@@ -14146,10 +14356,10 @@
         <v>259</v>
       </c>
       <c r="I50" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>11</v>
       </c>
@@ -14176,10 +14386,10 @@
         <v>259</v>
       </c>
       <c r="I51" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>11</v>
       </c>
@@ -14206,10 +14416,10 @@
         <v>259</v>
       </c>
       <c r="I52" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>11</v>
       </c>
@@ -14236,10 +14446,10 @@
         <v>259</v>
       </c>
       <c r="I53" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -14266,10 +14476,10 @@
         <v>259</v>
       </c>
       <c r="I54" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>11</v>
       </c>
@@ -14296,10 +14506,10 @@
         <v>259</v>
       </c>
       <c r="I55" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>13</v>
       </c>
@@ -14326,10 +14536,10 @@
         <v>259</v>
       </c>
       <c r="I56" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>13</v>
       </c>
@@ -14356,10 +14566,10 @@
         <v>259</v>
       </c>
       <c r="I57" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>13</v>
       </c>
@@ -14386,10 +14596,10 @@
         <v>259</v>
       </c>
       <c r="I58" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>13</v>
       </c>
@@ -14416,10 +14626,10 @@
         <v>259</v>
       </c>
       <c r="I59" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>14</v>
       </c>
@@ -14446,10 +14656,10 @@
         <v>259</v>
       </c>
       <c r="I60" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>14</v>
       </c>
@@ -14476,10 +14686,10 @@
         <v>259</v>
       </c>
       <c r="I61" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>14</v>
       </c>
@@ -14506,10 +14716,10 @@
         <v>259</v>
       </c>
       <c r="I62" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14</v>
       </c>
@@ -14536,10 +14746,10 @@
         <v>259</v>
       </c>
       <c r="I63" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>15</v>
       </c>
@@ -14566,10 +14776,10 @@
         <v>259</v>
       </c>
       <c r="I64" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>15</v>
       </c>
@@ -14596,10 +14806,10 @@
         <v>259</v>
       </c>
       <c r="I65" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>15</v>
       </c>
@@ -14626,10 +14836,10 @@
         <v>259</v>
       </c>
       <c r="I66" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>15</v>
       </c>
@@ -14656,10 +14866,10 @@
         <v>259</v>
       </c>
       <c r="I67" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>15</v>
       </c>
@@ -14686,10 +14896,10 @@
         <v>259</v>
       </c>
       <c r="I68" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>15</v>
       </c>
@@ -14716,10 +14926,10 @@
         <v>259</v>
       </c>
       <c r="I69" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>15</v>
       </c>
@@ -14746,10 +14956,10 @@
         <v>259</v>
       </c>
       <c r="I70" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>15</v>
       </c>
@@ -14776,10 +14986,10 @@
         <v>259</v>
       </c>
       <c r="I71" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>15</v>
       </c>
@@ -14806,10 +15016,10 @@
         <v>259</v>
       </c>
       <c r="I72" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>15</v>
       </c>
@@ -14836,10 +15046,10 @@
         <v>259</v>
       </c>
       <c r="I73" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15</v>
       </c>
@@ -14866,10 +15076,10 @@
         <v>259</v>
       </c>
       <c r="I74" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>15</v>
       </c>
@@ -14896,10 +15106,10 @@
         <v>259</v>
       </c>
       <c r="I75" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>15</v>
       </c>
@@ -14926,10 +15136,10 @@
         <v>259</v>
       </c>
       <c r="I76" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>15</v>
       </c>
@@ -14959,7 +15169,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>15</v>
       </c>
@@ -14989,7 +15199,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>15</v>
       </c>
@@ -15019,7 +15229,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>15</v>
       </c>
@@ -15049,7 +15259,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>16</v>
       </c>
@@ -15079,7 +15289,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>16</v>
       </c>
@@ -15109,7 +15319,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>16</v>
       </c>
@@ -15139,7 +15349,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>16</v>
       </c>
@@ -15169,7 +15379,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>16</v>
       </c>
@@ -15199,7 +15409,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>16</v>
       </c>
@@ -15229,7 +15439,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>16</v>
       </c>
@@ -15259,7 +15469,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>16</v>
       </c>
@@ -15289,7 +15499,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>16</v>
       </c>
@@ -15319,7 +15529,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>16</v>
       </c>
@@ -15349,7 +15559,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>16</v>
       </c>
@@ -15379,7 +15589,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>16</v>
       </c>
@@ -15409,7 +15619,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>16</v>
       </c>
@@ -15439,7 +15649,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>17</v>
       </c>
@@ -15469,7 +15679,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>17</v>
       </c>
@@ -15499,7 +15709,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>17</v>
       </c>
@@ -15529,7 +15739,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>17</v>
       </c>
@@ -15559,7 +15769,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>18</v>
       </c>
@@ -15589,7 +15799,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>18</v>
       </c>
@@ -15619,7 +15829,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>18</v>
       </c>
@@ -15649,7 +15859,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>19</v>
       </c>
@@ -15679,7 +15889,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20</v>
       </c>
@@ -15709,7 +15919,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>20</v>
       </c>
@@ -15739,7 +15949,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>20</v>
       </c>
@@ -15769,7 +15979,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>20</v>
       </c>
@@ -15799,7 +16009,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>20</v>
       </c>
@@ -15829,7 +16039,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>21</v>
       </c>
@@ -15859,7 +16069,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>21</v>
       </c>
@@ -15889,7 +16099,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>21</v>
       </c>
@@ -15919,7 +16129,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>21</v>
       </c>
@@ -15949,7 +16159,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>21</v>
       </c>
@@ -15979,7 +16189,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>22</v>
       </c>
@@ -16009,7 +16219,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>22</v>
       </c>
@@ -16039,7 +16249,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>22</v>
       </c>
@@ -16069,7 +16279,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>22</v>
       </c>
@@ -16099,7 +16309,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>22</v>
       </c>
@@ -16129,7 +16339,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>24</v>
       </c>
@@ -16159,7 +16369,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>24</v>
       </c>
@@ -16189,7 +16399,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>24</v>
       </c>
@@ -16219,7 +16429,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>24</v>
       </c>
@@ -16249,7 +16459,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>24</v>
       </c>
@@ -16279,7 +16489,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>25</v>
       </c>
@@ -16309,7 +16519,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>26</v>
       </c>
@@ -16339,7 +16549,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>26</v>
       </c>
@@ -16369,7 +16579,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>26</v>
       </c>
@@ -16399,7 +16609,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>26</v>
       </c>
@@ -16429,7 +16639,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>27</v>
       </c>
@@ -16459,7 +16669,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>27</v>
       </c>
@@ -16489,7 +16699,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>27</v>
       </c>
@@ -16519,7 +16729,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>27</v>
       </c>
@@ -16549,7 +16759,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>28</v>
       </c>
@@ -16579,7 +16789,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>29</v>
       </c>
@@ -16609,7 +16819,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>29</v>
       </c>
@@ -16639,7 +16849,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>29</v>
       </c>
@@ -16669,7 +16879,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>31</v>
       </c>
@@ -16699,7 +16909,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>31</v>
       </c>
@@ -16729,7 +16939,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>31</v>
       </c>
@@ -16759,7 +16969,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>32</v>
       </c>
@@ -16789,7 +16999,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>32</v>
       </c>
@@ -16819,7 +17029,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>32</v>
       </c>
@@ -16849,7 +17059,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>32</v>
       </c>
@@ -16879,7 +17089,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>32</v>
       </c>
@@ -16909,7 +17119,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>32</v>
       </c>
@@ -16939,7 +17149,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>32</v>
       </c>
@@ -16969,7 +17179,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>32</v>
       </c>
@@ -16999,7 +17209,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>32</v>
       </c>
@@ -17029,7 +17239,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>32</v>
       </c>
@@ -17059,7 +17269,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>32</v>
       </c>
@@ -17089,7 +17299,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>32</v>
       </c>
@@ -17119,7 +17329,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>32</v>
       </c>
@@ -17149,7 +17359,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>32</v>
       </c>
@@ -17179,7 +17389,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>32</v>
       </c>
@@ -17209,7 +17419,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>32</v>
       </c>
@@ -17239,7 +17449,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>32</v>
       </c>
@@ -17269,7 +17479,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>32</v>
       </c>
@@ -17299,7 +17509,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>32</v>
       </c>
@@ -17329,7 +17539,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>32</v>
       </c>
@@ -17359,7 +17569,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>32</v>
       </c>
@@ -17389,7 +17599,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>32</v>
       </c>
@@ -17419,7 +17629,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>32</v>
       </c>
@@ -17449,7 +17659,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>32</v>
       </c>
@@ -17479,7 +17689,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>33</v>
       </c>
@@ -17509,7 +17719,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>33</v>
       </c>
@@ -17539,7 +17749,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>33</v>
       </c>
@@ -17569,7 +17779,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>33</v>
       </c>
@@ -17599,7 +17809,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>34</v>
       </c>
@@ -17629,7 +17839,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>34</v>
       </c>
@@ -17659,7 +17869,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>34</v>
       </c>
@@ -17689,7 +17899,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>34</v>
       </c>
@@ -17719,7 +17929,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>37</v>
       </c>
@@ -17746,7 +17956,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>37</v>
       </c>
@@ -17776,7 +17986,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>37</v>
       </c>
@@ -17806,7 +18016,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>37</v>
       </c>
@@ -17836,7 +18046,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>37</v>
       </c>
@@ -17866,7 +18076,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>37</v>
       </c>
@@ -17896,7 +18106,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>37</v>
       </c>
@@ -17926,7 +18136,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>37</v>
       </c>
@@ -17953,10 +18163,10 @@
         <v>259</v>
       </c>
       <c r="I177" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>38</v>
       </c>
@@ -17983,10 +18193,10 @@
         <v>259</v>
       </c>
       <c r="I178" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>38</v>
       </c>
@@ -18013,10 +18223,10 @@
         <v>259</v>
       </c>
       <c r="I179" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>43</v>
       </c>
@@ -18043,10 +18253,10 @@
         <v>259</v>
       </c>
       <c r="I180" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>43</v>
       </c>
@@ -18073,10 +18283,10 @@
         <v>259</v>
       </c>
       <c r="I181" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>43</v>
       </c>
@@ -18103,10 +18313,10 @@
         <v>259</v>
       </c>
       <c r="I182" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>45</v>
       </c>
@@ -18133,10 +18343,10 @@
         <v>259</v>
       </c>
       <c r="I183" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>45</v>
       </c>
@@ -18163,10 +18373,10 @@
         <v>259</v>
       </c>
       <c r="I184" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>45</v>
       </c>
@@ -18193,10 +18403,10 @@
         <v>259</v>
       </c>
       <c r="I185" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>45</v>
       </c>
@@ -18223,10 +18433,10 @@
         <v>259</v>
       </c>
       <c r="I186" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>45</v>
       </c>
@@ -18253,10 +18463,10 @@
         <v>259</v>
       </c>
       <c r="I187" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>46</v>
       </c>
@@ -18283,10 +18493,10 @@
         <v>259</v>
       </c>
       <c r="I188" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>46</v>
       </c>
@@ -18310,10 +18520,10 @@
         <v>259</v>
       </c>
       <c r="I189" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>46</v>
       </c>
@@ -18340,10 +18550,10 @@
         <v>259</v>
       </c>
       <c r="I190" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>48</v>
       </c>
@@ -18370,10 +18580,10 @@
         <v>259</v>
       </c>
       <c r="I191" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>48</v>
       </c>
@@ -18400,10 +18610,10 @@
         <v>259</v>
       </c>
       <c r="I192" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>48</v>
       </c>
@@ -18430,10 +18640,10 @@
         <v>259</v>
       </c>
       <c r="I193" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>48</v>
       </c>
@@ -18460,10 +18670,10 @@
         <v>259</v>
       </c>
       <c r="I194" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>48</v>
       </c>
@@ -18490,10 +18700,10 @@
         <v>259</v>
       </c>
       <c r="I195" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>48</v>
       </c>
@@ -18517,10 +18727,10 @@
         <v>259</v>
       </c>
       <c r="I196" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>49</v>
       </c>
@@ -18547,10 +18757,10 @@
         <v>259</v>
       </c>
       <c r="I197" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>49</v>
       </c>
@@ -18577,10 +18787,10 @@
         <v>259</v>
       </c>
       <c r="I198" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>50</v>
       </c>
@@ -18607,10 +18817,10 @@
         <v>259</v>
       </c>
       <c r="I199" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>50</v>
       </c>
@@ -18636,11 +18846,11 @@
       <c r="H200" t="s">
         <v>259</v>
       </c>
-      <c r="I200" s="4" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+      <c r="I200" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>50</v>
       </c>
@@ -18666,8 +18876,8 @@
       <c r="H201" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="I201" s="4" t="s">
-        <v>349</v>
+      <c r="I201" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>